<commit_message>
Output pairs to Excel file
</commit_message>
<xml_diff>
--- a/biglittlepreferences.xlsx
+++ b/biglittlepreferences.xlsx
@@ -1,73 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Bigs" sheetId="3" r:id="rId1"/>
-    <sheet name="Littles" sheetId="4" r:id="rId2"/>
+    <sheet name="Bigs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Littles" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Pairs" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Big 1</t>
   </si>
   <si>
+    <t>Little 2</t>
+  </si>
+  <si>
+    <t>Little 3</t>
+  </si>
+  <si>
+    <t>Little 5</t>
+  </si>
+  <si>
     <t>Big 2</t>
   </si>
   <si>
+    <t>Little 4</t>
+  </si>
+  <si>
     <t>Big 3</t>
   </si>
   <si>
+    <t>Little 1</t>
+  </si>
+  <si>
     <t>Big 4</t>
   </si>
   <si>
     <t>Big 5</t>
   </si>
   <si>
-    <t>Little 1</t>
-  </si>
-  <si>
-    <t>Little 2</t>
-  </si>
-  <si>
-    <t>Little 3</t>
-  </si>
-  <si>
-    <t>Little 4</t>
-  </si>
-  <si>
-    <t>Little 5</t>
+    <t>Bigs</t>
+  </si>
+  <si>
+    <t>Littles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -83,24 +86,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -400,171 +394,246 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Account for different number of bigs and littles
</commit_message>
<xml_diff>
--- a/biglittlepreferences.xlsx
+++ b/biglittlepreferences.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Big 1</t>
   </si>
@@ -48,10 +48,16 @@
     <t>Big 5</t>
   </si>
   <si>
+    <t>Little 6</t>
+  </si>
+  <si>
     <t>Bigs</t>
   </si>
   <si>
     <t>Littles</t>
+  </si>
+  <si>
+    <t>Big 1*</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -564,6 +570,20 @@
       </c>
       <c r="D5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,10 +607,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -619,18 +639,26 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change spreadsheet position from which data is grabbed
This change was specifically implemented to reflect the structure of
the format of a google form responses .csv download.
</commit_message>
<xml_diff>
--- a/biglittlepreferences.xlsx
+++ b/biglittlepreferences.xlsx
@@ -1,54 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Programming\StableMarriage\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Bigs" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Littles" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Pairs" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Bigs" sheetId="1" r:id="rId1"/>
+    <sheet name="Littles" sheetId="2" r:id="rId2"/>
+    <sheet name="Pairs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
-  <si>
-    <t>Big 1</t>
-  </si>
-  <si>
-    <t>Little 2</t>
-  </si>
-  <si>
-    <t>Little 3</t>
-  </si>
-  <si>
-    <t>Little 5</t>
-  </si>
-  <si>
-    <t>Big 2</t>
-  </si>
-  <si>
-    <t>Little 4</t>
-  </si>
-  <si>
-    <t>Big 3</t>
-  </si>
-  <si>
-    <t>Little 1</t>
-  </si>
-  <si>
-    <t>Big 4</t>
-  </si>
-  <si>
-    <t>Big 5</t>
-  </si>
-  <si>
-    <t>Little 6</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Preferred Little #1</t>
+  </si>
+  <si>
+    <t>Preferred Little #2</t>
+  </si>
+  <si>
+    <t>Preferred Little #3</t>
+  </si>
+  <si>
+    <t>2016/10/06 8:26:24 PM AST</t>
+  </si>
+  <si>
+    <t>David Zhao</t>
+  </si>
+  <si>
+    <t>Capitol Hillary Clinton</t>
+  </si>
+  <si>
+    <t>Ernie and Bert Sanders</t>
+  </si>
+  <si>
+    <t>Ben Cars- My Luggage</t>
+  </si>
+  <si>
+    <t>2016/10/06 8:30:39 PM AST</t>
+  </si>
+  <si>
+    <t>Disha Jain</t>
+  </si>
+  <si>
+    <t>Parry Hotter</t>
+  </si>
+  <si>
+    <t>Her Mine E</t>
+  </si>
+  <si>
+    <t>Ron Ferretly</t>
+  </si>
+  <si>
+    <t>2016/10/06 8:33:35 PM AST</t>
+  </si>
+  <si>
+    <t>Robyn Guarriello</t>
+  </si>
+  <si>
+    <t>2016/10/06 8:39:12 PM AST</t>
+  </si>
+  <si>
+    <t>Rohni Awasthi</t>
+  </si>
+  <si>
+    <t>Larry David</t>
+  </si>
+  <si>
+    <t>Larry Richards</t>
+  </si>
+  <si>
+    <t>2016/10/06 8:41:50 PM AST</t>
+  </si>
+  <si>
+    <t>Shirali Nigam</t>
+  </si>
+  <si>
+    <t>Preferred Big #1</t>
+  </si>
+  <si>
+    <t>Preferred Big #2</t>
+  </si>
+  <si>
+    <t>Preferred Big #3</t>
   </si>
   <si>
     <t>Bigs</t>
@@ -57,26 +107,31 @@
     <t>Littles</t>
   </si>
   <si>
-    <t>Big 1*</t>
+    <t>Disha Jain*</t>
+  </si>
+  <si>
+    <t>David Zhao*</t>
+  </si>
+  <si>
+    <t>Robyn Guarriello*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -92,15 +147,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,20 +464,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,242 +486,348 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allow input from two csv files
The previous commit description falsely assumed the Google Form download
.csv file could be parsed the same way as an .xlsx. This two-csv file
input directly mirrors the outputs of two Google Forms for bigs
preferences and littles preferences.
</commit_message>
<xml_diff>
--- a/biglittlepreferences.xlsx
+++ b/biglittlepreferences.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Programming\StableMarriage\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Bigs" sheetId="1" r:id="rId1"/>
-    <sheet name="Littles" sheetId="2" r:id="rId2"/>
-    <sheet name="Pairs" sheetId="3" r:id="rId3"/>
+    <sheet name="Bigs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Littles" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Pairs" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Timestamp</t>
   </si>
@@ -107,10 +102,10 @@
     <t>Littles</t>
   </si>
   <si>
+    <t>David Zhao*</t>
+  </si>
+  <si>
     <t>Disha Jain*</t>
-  </si>
-  <si>
-    <t>David Zhao*</t>
   </si>
   <si>
     <t>Robyn Guarriello*</t>
@@ -119,19 +114,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -147,24 +143,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -464,16 +451,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -507,7 +498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -524,7 +515,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -541,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -555,7 +546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -573,21 +564,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +599,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -621,7 +616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -638,7 +633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -655,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -672,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -689,7 +684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -706,7 +701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -723,7 +718,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -741,21 +736,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -763,7 +762,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -771,15 +770,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -787,39 +786,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -828,6 +827,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>